<commit_message>
Between Date Validation applied. Save and Print Files are under progress and soon will be completed. All Files Finished placing in respective folders
</commit_message>
<xml_diff>
--- a/Reports/Templates/FreqAccTestTemplate.xlsx
+++ b/Reports/Templates/FreqAccTestTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaswa\PycharmProjects\ATEC1\DataBase\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaswa\PycharmProjects\ATEC1\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF6D139-0A66-4C48-B78E-08C34BA10302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52082E84-C82A-4624-9F74-C1EA0FC25B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,10 +480,70 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -494,66 +554,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,8 +851,8 @@
     <col min="6" max="6" width="19.42578125" style="14" customWidth="1"/>
     <col min="7" max="7" width="2.42578125" style="14" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" style="14" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" style="2" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -927,10 +927,10 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="29"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="6" t="s">
         <v>1</v>
       </c>
@@ -941,14 +941,14 @@
       <c r="G8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="25"/>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="29"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="6" t="s">
         <v>1</v>
       </c>
@@ -975,22 +975,22 @@
       <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="27"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="47"/>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="29"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="6" t="s">
         <v>1</v>
       </c>
@@ -1001,14 +1001,14 @@
       <c r="G12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="25"/>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="29"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="6" t="s">
         <v>1</v>
       </c>
@@ -1019,14 +1019,14 @@
       <c r="G13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="25"/>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="29"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="6" t="s">
         <v>1</v>
       </c>
@@ -1037,14 +1037,14 @@
       <c r="G14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="23"/>
-      <c r="I14" s="24"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="25"/>
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="29"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="6" t="s">
         <v>1</v>
       </c>
@@ -1057,8 +1057,8 @@
       <c r="G15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="23"/>
-      <c r="I15" s="24"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="25"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
@@ -1075,74 +1075,63 @@
       <c r="B17" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45" t="s">
+      <c r="D17" s="28"/>
+      <c r="E17" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45" t="s">
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="45"/>
+      <c r="I17" s="28"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="13">
         <v>1</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
     </row>
     <row r="19" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="13">
         <v>2</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="13">
         <v>3</v>
       </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="24"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="C2:H2"/>
@@ -1154,13 +1143,24 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="F5:I5"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
   </mergeCells>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>